<commit_message>
El assembler ahora lee xlsx
</commit_message>
<xml_diff>
--- a/Instrucciones-computador.xlsx
+++ b/Instrucciones-computador.xlsx
@@ -4,7 +4,7 @@
   <workbookPr/>
   <sheets>
     <sheet state="visible" name="Etapa 1" sheetId="1" r:id="rId4"/>
-    <sheet state="visible" name="Etapa 2" sheetId="2" r:id="rId5"/>
+    <sheet state="visible" name="Etapa-2" sheetId="2" r:id="rId5"/>
     <sheet state="visible" name="Datos" sheetId="3" r:id="rId6"/>
     <sheet state="visible" name="ALU" sheetId="4" r:id="rId7"/>
   </sheets>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="643" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="126">
   <si>
     <t>Assambler inst</t>
   </si>
@@ -288,7 +288,7 @@
     <t>guarda Mem[SP] en PC</t>
   </si>
   <si>
-    <t xml:space="preserve">PUSH A </t>
+    <t>PUSH A</t>
   </si>
   <si>
     <t>PUSH</t>
@@ -8050,7 +8050,7 @@
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JNE </v>
+        <v>JNE Ins</v>
       </c>
       <c r="B66" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8058,6 +8058,9 @@
       </c>
       <c r="C66" s="2" t="s">
         <v>51</v>
+      </c>
+      <c r="D66" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
@@ -8157,7 +8160,7 @@
     <row r="67" ht="15.75" customHeight="1">
       <c r="A67" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JGT </v>
+        <v>JGT Ins</v>
       </c>
       <c r="B67" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8165,6 +8168,9 @@
       </c>
       <c r="C67" s="2" t="s">
         <v>52</v>
+      </c>
+      <c r="D67" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
@@ -8264,7 +8270,7 @@
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JLT </v>
+        <v>JLT Ins</v>
       </c>
       <c r="B68" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8272,6 +8278,9 @@
       </c>
       <c r="C68" s="2" t="s">
         <v>53</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F68" s="3"/>
       <c r="G68" s="3"/>
@@ -8371,7 +8380,7 @@
     <row r="69" ht="15.75" customHeight="1">
       <c r="A69" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JGE </v>
+        <v>JGE Ins</v>
       </c>
       <c r="B69" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8379,6 +8388,9 @@
       </c>
       <c r="C69" s="2" t="s">
         <v>54</v>
+      </c>
+      <c r="D69" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F69" s="3"/>
       <c r="G69" s="3"/>
@@ -8478,7 +8490,7 @@
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JLE </v>
+        <v>JLE Ins</v>
       </c>
       <c r="B70" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8486,6 +8498,9 @@
       </c>
       <c r="C70" s="2" t="s">
         <v>55</v>
+      </c>
+      <c r="D70" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -8585,7 +8600,7 @@
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="2" t="str">
         <f t="shared" si="13"/>
-        <v>JCR </v>
+        <v>JCR Ins</v>
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" si="4"/>
@@ -8593,6 +8608,9 @@
       </c>
       <c r="C71" s="2" t="s">
         <v>56</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="F71" s="3"/>
       <c r="G71" s="3"/>

</xml_diff>

<commit_message>
con if en vez de match
</commit_message>
<xml_diff>
--- a/Instrucciones-computador.xlsx
+++ b/Instrucciones-computador.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="684" uniqueCount="131">
   <si>
     <t>Assambler inst</t>
   </si>
@@ -201,10 +201,22 @@
     <t>Op2</t>
   </si>
   <si>
+    <t>Funciona</t>
+  </si>
+  <si>
+    <t>PROBLEMA ASSEMBLY</t>
+  </si>
+  <si>
     <t>MOV A,(B)</t>
   </si>
   <si>
     <t>(B)</t>
+  </si>
+  <si>
+    <t>NO</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
   <si>
     <t>Entrega 2</t>
@@ -268,6 +280,9 @@
   </si>
   <si>
     <t>sub A,1</t>
+  </si>
+  <si>
+    <t>SALTA 1 VEZ, las consecutivas no las hace</t>
   </si>
   <si>
     <t>CALL Dir</t>
@@ -535,6 +550,9 @@
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="3" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
@@ -548,9 +566,6 @@
     <xf borderId="0" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1" applyFont="1"/>
     <xf borderId="1" fillId="5" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -571,7 +586,18 @@
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border/>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -9706,6 +9732,8 @@
     <col customWidth="1" min="23" max="23" width="2.57"/>
     <col customWidth="1" min="24" max="24" width="2.71"/>
     <col customWidth="1" min="25" max="25" width="2.57"/>
+    <col customWidth="1" min="26" max="26" width="20.71"/>
+    <col customWidth="1" min="27" max="27" width="22.43"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -9837,6 +9865,12 @@
       <c r="Y2" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="Z2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="str">
@@ -9910,9 +9944,12 @@
       <c r="Y3" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z3" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA3" s="4"/>
-      <c r="AB3" s="3"/>
-      <c r="AC3" s="4"/>
+      <c r="AB3" s="4"/>
+      <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
     <row r="4">
@@ -9993,9 +10030,11 @@
       <c r="Y4" s="4">
         <v>0.0</v>
       </c>
-      <c r="Z4" s="4"/>
+      <c r="Z4" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA4" s="3"/>
-      <c r="AC4" s="3"/>
+      <c r="AB4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
     <row r="5">
@@ -10076,8 +10115,11 @@
       <c r="Y5" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z5" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA5" s="3"/>
-      <c r="AC5" s="3"/>
+      <c r="AB5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
     <row r="6">
@@ -10158,8 +10200,11 @@
       <c r="Y6" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z6" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA6" s="3"/>
-      <c r="AC6" s="3"/>
+      <c r="AB6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
     <row r="7">
@@ -10240,8 +10285,11 @@
       <c r="Y7" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z7" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA7" s="3"/>
-      <c r="AC7" s="3"/>
+      <c r="AB7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
     <row r="8">
@@ -10322,7 +10370,10 @@
       <c r="Y8" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC8" s="3"/>
+      <c r="Z8" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA8" s="3"/>
       <c r="AD8" s="3"/>
     </row>
     <row r="9">
@@ -10403,7 +10454,10 @@
       <c r="Y9" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC9" s="3"/>
+      <c r="Z9" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA9" s="3"/>
       <c r="AD9" s="3"/>
     </row>
     <row r="10">
@@ -10484,7 +10538,10 @@
       <c r="Y10" s="3">
         <v>1.0</v>
       </c>
-      <c r="AC10" s="3"/>
+      <c r="Z10" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA10" s="3"/>
       <c r="AD10" s="3"/>
     </row>
     <row r="11">
@@ -10565,12 +10622,15 @@
       <c r="Y11" s="2">
         <v>1.0</v>
       </c>
-      <c r="AC11" s="3"/>
+      <c r="Z11" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA11" s="3"/>
       <c r="AD11" s="3"/>
     </row>
     <row r="12">
       <c r="A12" s="1" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B12" s="2" t="str">
         <f t="shared" si="1"/>
@@ -10583,7 +10643,7 @@
         <v>28</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F12" s="9">
         <v>0.0</v>
@@ -10645,15 +10705,20 @@
       <c r="Y12" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA12" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC12" s="3"/>
+      <c r="Z12" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA12" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB12" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD12" s="3"/>
     </row>
     <row r="13">
       <c r="A13" s="1" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B13" s="2" t="str">
         <f t="shared" si="1"/>
@@ -10666,7 +10731,7 @@
         <v>29</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F13" s="9">
         <v>0.0</v>
@@ -10728,15 +10793,20 @@
       <c r="Y13" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA13" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC13" s="3"/>
+      <c r="Z13" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA13" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB13" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD13" s="3"/>
     </row>
     <row r="14">
       <c r="A14" s="1" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="B14" s="2" t="str">
         <f t="shared" si="1"/>
@@ -10746,7 +10816,7 @@
         <v>27</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>28</v>
@@ -10811,10 +10881,15 @@
       <c r="Y14" s="1">
         <v>1.0</v>
       </c>
-      <c r="AA14" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC14" s="3"/>
+      <c r="Z14" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA14" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB14" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD14" s="3"/>
     </row>
     <row r="15">
@@ -10888,14 +10963,18 @@
       <c r="Y15" s="11">
         <v>1.0</v>
       </c>
-      <c r="Z15" s="12"/>
-      <c r="AA15" s="11" t="s">
-        <v>62</v>
+      <c r="Z15" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA15" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="AB15" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="AC15" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="AC15" s="11" t="s">
+        <v>69</v>
+      </c>
       <c r="AD15" s="3"/>
     </row>
     <row r="16">
@@ -10976,8 +11055,11 @@
       <c r="Y16" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z16" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA16" s="3"/>
-      <c r="AC16" s="3"/>
+      <c r="AB16" s="3"/>
       <c r="AD16" s="3"/>
     </row>
     <row r="17">
@@ -11058,8 +11140,11 @@
       <c r="Y17" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z17" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA17" s="3"/>
-      <c r="AC17" s="3"/>
+      <c r="AB17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
     <row r="18">
@@ -11140,8 +11225,11 @@
       <c r="Y18" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z18" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA18" s="3"/>
-      <c r="AC18" s="3"/>
+      <c r="AB18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
     <row r="19">
@@ -11218,12 +11306,14 @@
       <c r="Y19" s="12">
         <v>0.0</v>
       </c>
-      <c r="Z19" s="12"/>
-      <c r="AA19" s="10"/>
-      <c r="AB19" s="11" t="s">
+      <c r="Z19" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA19" s="3"/>
+      <c r="AB19" s="10"/>
+      <c r="AC19" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
     <row r="20">
@@ -11304,7 +11394,10 @@
       <c r="Y20" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC20" s="3"/>
+      <c r="Z20" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
     <row r="21">
@@ -11381,12 +11474,14 @@
       <c r="Y21" s="15">
         <v>0.0</v>
       </c>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="11" t="s">
+      <c r="Z21" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="15"/>
+      <c r="AC21" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
     <row r="22">
@@ -11464,13 +11559,16 @@
       <c r="Y22" s="2">
         <v>1.0</v>
       </c>
+      <c r="Z22" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA22" s="3"/>
-      <c r="AC22" s="3"/>
+      <c r="AB22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>66</v>
+        <v>70</v>
       </c>
       <c r="B23" s="2" t="str">
         <f t="shared" si="1"/>
@@ -11483,7 +11581,7 @@
         <v>28</v>
       </c>
       <c r="E23" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F23" s="9">
         <v>0.0</v>
@@ -11545,15 +11643,20 @@
       <c r="Y23" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA23" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC23" s="3"/>
+      <c r="Z23" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA23" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD23" s="3"/>
     </row>
     <row r="24">
       <c r="A24" s="11" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="B24" s="12" t="str">
         <f t="shared" si="1"/>
@@ -11566,7 +11669,7 @@
         <v>29</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F24" s="13">
         <v>0.0</v>
@@ -11624,12 +11727,14 @@
       <c r="Y24" s="11">
         <v>0.0</v>
       </c>
-      <c r="Z24" s="12"/>
-      <c r="AA24" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB24" s="12"/>
-      <c r="AC24" s="3"/>
+      <c r="Z24" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC24" s="12"/>
       <c r="AD24" s="3"/>
     </row>
     <row r="25">
@@ -11711,8 +11816,11 @@
       <c r="Y25" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z25" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA25" s="3"/>
-      <c r="AC25" s="3"/>
+      <c r="AB25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
     <row r="26">
@@ -11794,8 +11902,11 @@
       <c r="Y26" s="2">
         <v>0.0</v>
       </c>
-      <c r="AA26" s="3"/>
-      <c r="AC26" s="3"/>
+      <c r="Z26" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA26" s="9"/>
+      <c r="AB26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
     <row r="27">
@@ -11877,8 +11988,11 @@
       <c r="Y27" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z27" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA27" s="3"/>
-      <c r="AC27" s="3"/>
+      <c r="AB27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
     <row r="28">
@@ -11939,8 +12053,8 @@
       <c r="R28" s="16">
         <v>1.0</v>
       </c>
-      <c r="S28" s="19"/>
-      <c r="T28" s="19"/>
+      <c r="S28" s="20"/>
+      <c r="T28" s="20"/>
       <c r="U28" s="16">
         <v>1.0</v>
       </c>
@@ -11956,12 +12070,16 @@
       <c r="Y28" s="15">
         <v>0.0</v>
       </c>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="18"/>
-      <c r="AB28" s="11" t="s">
+      <c r="Z28" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA28" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB28" s="18"/>
+      <c r="AC28" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
     <row r="29">
@@ -12043,7 +12161,10 @@
       <c r="Y29" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC29" s="3"/>
+      <c r="Z29" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA29" s="3"/>
       <c r="AD29" s="3"/>
     </row>
     <row r="30">
@@ -12122,11 +12243,11 @@
         <v>0.0</v>
       </c>
       <c r="Z30" s="12"/>
-      <c r="AA30" s="12"/>
-      <c r="AB30" s="11" t="s">
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="12"/>
+      <c r="AC30" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
     <row r="31">
@@ -12205,13 +12326,16 @@
       <c r="Y31" s="2">
         <v>1.0</v>
       </c>
+      <c r="Z31" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA31" s="3"/>
-      <c r="AC31" s="3"/>
+      <c r="AB31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
     <row r="32">
       <c r="A32" s="1" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B32" s="2" t="str">
         <f t="shared" si="1"/>
@@ -12224,7 +12348,7 @@
         <v>28</v>
       </c>
       <c r="E32" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F32" s="9">
         <v>0.0</v>
@@ -12286,15 +12410,20 @@
       <c r="Y32" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA32" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC32" s="3"/>
+      <c r="Z32" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA32" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD32" s="3"/>
     </row>
     <row r="33">
       <c r="A33" s="11" t="s">
-        <v>69</v>
+        <v>73</v>
       </c>
       <c r="B33" s="12" t="str">
         <f t="shared" si="1"/>
@@ -12307,7 +12436,7 @@
         <v>29</v>
       </c>
       <c r="E33" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F33" s="13">
         <v>0.0</v>
@@ -12361,12 +12490,16 @@
       <c r="Y33" s="11">
         <v>0.0</v>
       </c>
-      <c r="Z33" s="12"/>
-      <c r="AA33" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB33" s="12"/>
-      <c r="AC33" s="3"/>
+      <c r="Z33" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA33" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB33" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC33" s="12"/>
       <c r="AD33" s="3"/>
     </row>
     <row r="34">
@@ -12448,8 +12581,11 @@
       <c r="Y34" s="2">
         <v>0.0</v>
       </c>
-      <c r="AA34" s="3"/>
-      <c r="AC34" s="3"/>
+      <c r="Z34" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA34" s="9"/>
+      <c r="AB34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
     <row r="35">
@@ -12531,8 +12667,11 @@
       <c r="Y35" s="2">
         <v>0.0</v>
       </c>
-      <c r="AA35" s="3"/>
-      <c r="AC35" s="3"/>
+      <c r="Z35" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA35" s="9"/>
+      <c r="AB35" s="3"/>
       <c r="AD35" s="3"/>
     </row>
     <row r="36">
@@ -12614,8 +12753,11 @@
       <c r="Y36" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z36" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA36" s="3"/>
-      <c r="AC36" s="3"/>
+      <c r="AB36" s="3"/>
       <c r="AD36" s="3"/>
     </row>
     <row r="37">
@@ -12676,8 +12818,8 @@
       <c r="R37" s="16">
         <v>0.0</v>
       </c>
-      <c r="S37" s="19"/>
-      <c r="T37" s="19"/>
+      <c r="S37" s="20"/>
+      <c r="T37" s="20"/>
       <c r="U37" s="16">
         <v>1.0</v>
       </c>
@@ -12693,12 +12835,16 @@
       <c r="Y37" s="15">
         <v>0.0</v>
       </c>
-      <c r="Z37" s="15"/>
-      <c r="AA37" s="18"/>
-      <c r="AB37" s="11" t="s">
+      <c r="Z37" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA37" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB37" s="18"/>
+      <c r="AC37" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
     </row>
     <row r="38">
@@ -12780,7 +12926,10 @@
       <c r="Y38" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC38" s="3"/>
+      <c r="Z38" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
     <row r="39">
@@ -12858,12 +13007,16 @@
       <c r="Y39" s="12">
         <v>0.0</v>
       </c>
-      <c r="Z39" s="12"/>
-      <c r="AA39" s="12"/>
-      <c r="AB39" s="11" t="s">
+      <c r="Z39" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA39" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB39" s="12"/>
+      <c r="AC39" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
     </row>
     <row r="40">
@@ -12942,13 +13095,16 @@
       <c r="Y40" s="2">
         <v>1.0</v>
       </c>
+      <c r="Z40" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA40" s="3"/>
-      <c r="AC40" s="3"/>
+      <c r="AB40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
     <row r="41">
       <c r="A41" s="1" t="s">
-        <v>70</v>
+        <v>74</v>
       </c>
       <c r="B41" s="2" t="str">
         <f t="shared" si="1"/>
@@ -12961,7 +13117,7 @@
         <v>28</v>
       </c>
       <c r="E41" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F41" s="9">
         <v>0.0</v>
@@ -13023,15 +13179,20 @@
       <c r="Y41" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA41" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC41" s="3"/>
+      <c r="Z41" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA41" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB41" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD41" s="3"/>
     </row>
     <row r="42">
       <c r="A42" s="11" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="B42" s="12" t="str">
         <f t="shared" si="1"/>
@@ -13044,7 +13205,7 @@
         <v>29</v>
       </c>
       <c r="E42" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F42" s="13">
         <v>0.0</v>
@@ -13099,14 +13260,18 @@
       <c r="Y42" s="11">
         <v>0.0</v>
       </c>
-      <c r="Z42" s="12"/>
-      <c r="AA42" s="11" t="s">
-        <v>62</v>
+      <c r="Z42" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA42" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="AB42" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="AC42" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
     <row r="43">
@@ -13188,8 +13353,11 @@
       <c r="Y43" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z43" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA43" s="3"/>
-      <c r="AC43" s="3"/>
+      <c r="AB43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
     <row r="44">
@@ -13271,8 +13439,11 @@
       <c r="Y44" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z44" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA44" s="3"/>
-      <c r="AC44" s="3"/>
+      <c r="AB44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
     <row r="45">
@@ -13354,8 +13525,11 @@
       <c r="Y45" s="2">
         <v>0.0</v>
       </c>
+      <c r="Z45" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA45" s="3"/>
-      <c r="AC45" s="3"/>
+      <c r="AB45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
     <row r="46">
@@ -13416,8 +13590,8 @@
       <c r="R46" s="16">
         <v>1.0</v>
       </c>
-      <c r="S46" s="19"/>
-      <c r="T46" s="19"/>
+      <c r="S46" s="20"/>
+      <c r="T46" s="20"/>
       <c r="U46" s="16">
         <v>1.0</v>
       </c>
@@ -13433,12 +13607,14 @@
       <c r="Y46" s="15">
         <v>0.0</v>
       </c>
-      <c r="Z46" s="15"/>
-      <c r="AA46" s="18"/>
-      <c r="AB46" s="11" t="s">
+      <c r="Z46" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="18"/>
+      <c r="AC46" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
     <row r="47">
@@ -13520,7 +13696,10 @@
       <c r="Y47" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC47" s="3"/>
+      <c r="Z47" s="1">
+        <v>1.0</v>
+      </c>
+      <c r="AA47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
     <row r="48">
@@ -13599,11 +13778,11 @@
         <v>0.0</v>
       </c>
       <c r="Z48" s="12"/>
-      <c r="AA48" s="12"/>
-      <c r="AB48" s="11" t="s">
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="12"/>
+      <c r="AC48" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
     <row r="49">
@@ -13682,13 +13861,16 @@
       <c r="Y49" s="2">
         <v>1.0</v>
       </c>
+      <c r="Z49" s="1">
+        <v>1.0</v>
+      </c>
       <c r="AA49" s="3"/>
-      <c r="AC49" s="3"/>
+      <c r="AB49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
     <row r="50">
       <c r="A50" s="1" t="s">
-        <v>72</v>
+        <v>76</v>
       </c>
       <c r="B50" s="2" t="str">
         <f t="shared" si="1"/>
@@ -13701,7 +13883,7 @@
         <v>28</v>
       </c>
       <c r="E50" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F50" s="9">
         <v>0.0</v>
@@ -13764,15 +13946,20 @@
       <c r="Y50" s="1">
         <v>0.0</v>
       </c>
-      <c r="AA50" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="AC50" s="3"/>
+      <c r="Z50" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA50" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB50" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="AD50" s="3"/>
     </row>
     <row r="51">
       <c r="A51" s="11" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="B51" s="12" t="str">
         <f t="shared" si="1"/>
@@ -13785,7 +13972,7 @@
         <v>29</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F51" s="13">
         <v>0.0</v>
@@ -13844,14 +14031,18 @@
       <c r="Y51" s="11">
         <v>0.0</v>
       </c>
-      <c r="Z51" s="12"/>
-      <c r="AA51" s="11" t="s">
-        <v>62</v>
+      <c r="Z51" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="AA51" s="9" t="s">
+        <v>65</v>
       </c>
       <c r="AB51" s="11" t="s">
-        <v>74</v>
-      </c>
-      <c r="AC51" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="AC51" s="11" t="s">
+        <v>78</v>
+      </c>
       <c r="AD51" s="3"/>
     </row>
     <row r="52">
@@ -13934,7 +14125,7 @@
         <v>0.0</v>
       </c>
       <c r="AA52" s="3"/>
-      <c r="AC52" s="3"/>
+      <c r="AB52" s="3"/>
       <c r="AD52" s="3"/>
     </row>
     <row r="53">
@@ -14017,7 +14208,7 @@
         <v>0.0</v>
       </c>
       <c r="AA53" s="3"/>
-      <c r="AC53" s="3"/>
+      <c r="AB53" s="3"/>
       <c r="AD53" s="3"/>
     </row>
     <row r="54">
@@ -14100,7 +14291,7 @@
         <v>0.0</v>
       </c>
       <c r="AA54" s="3"/>
-      <c r="AC54" s="3"/>
+      <c r="AB54" s="3"/>
       <c r="AD54" s="3"/>
     </row>
     <row r="55">
@@ -14179,11 +14370,11 @@
         <v>0.0</v>
       </c>
       <c r="Z55" s="12"/>
-      <c r="AA55" s="10"/>
-      <c r="AB55" s="11" t="s">
+      <c r="AA55" s="3"/>
+      <c r="AB55" s="10"/>
+      <c r="AC55" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
     </row>
     <row r="56">
@@ -14265,7 +14456,7 @@
       <c r="Y56" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC56" s="3"/>
+      <c r="AA56" s="3"/>
       <c r="AD56" s="3"/>
     </row>
     <row r="57">
@@ -14344,11 +14535,11 @@
         <v>0.0</v>
       </c>
       <c r="Z57" s="12"/>
-      <c r="AA57" s="12"/>
-      <c r="AB57" s="11" t="s">
+      <c r="AA57" s="3"/>
+      <c r="AB57" s="12"/>
+      <c r="AC57" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
     </row>
     <row r="58">
@@ -14428,12 +14619,12 @@
         <v>1.0</v>
       </c>
       <c r="AA58" s="3"/>
-      <c r="AC58" s="3"/>
+      <c r="AB58" s="3"/>
       <c r="AD58" s="3"/>
     </row>
     <row r="59">
       <c r="A59" s="1" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="B59" s="2" t="str">
         <f t="shared" si="1"/>
@@ -14446,7 +14637,7 @@
         <v>28</v>
       </c>
       <c r="E59" s="9" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F59" s="9">
         <v>0.0</v>
@@ -14510,12 +14701,12 @@
         <v>0.0</v>
       </c>
       <c r="AA59" s="3"/>
-      <c r="AC59" s="3"/>
+      <c r="AB59" s="3"/>
       <c r="AD59" s="3"/>
     </row>
     <row r="60">
       <c r="A60" s="11" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B60" s="12" t="str">
         <f t="shared" si="1"/>
@@ -14528,7 +14719,7 @@
         <v>29</v>
       </c>
       <c r="E60" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F60" s="13">
         <v>0.0</v>
@@ -14588,99 +14779,98 @@
         <v>0.0</v>
       </c>
       <c r="Z60" s="11"/>
-      <c r="AA60" s="10"/>
-      <c r="AB60" s="12"/>
-      <c r="AC60" s="3"/>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="10"/>
+      <c r="AC60" s="12"/>
       <c r="AD60" s="3"/>
     </row>
     <row r="61">
-      <c r="A61" s="20" t="str">
-        <f t="shared" ref="A61:A69" si="8">CONCATENATE(C61," ",D61,", ",E61)</f>
-        <v>NOT A, </v>
-      </c>
-      <c r="B61" s="20" t="str">
+      <c r="A61" s="21" t="str">
+        <f>CONCATENATE(C61," ",D61)</f>
+        <v>NOT A</v>
+      </c>
+      <c r="B61" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00000000001011000100</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E61" s="21"/>
-      <c r="F61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="J61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="K61" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L61" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M61" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N61" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O61" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P61" s="20">
+      <c r="E61" s="22"/>
+      <c r="F61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="J61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="K61" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L61" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M61" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N61" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O61" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P61" s="21">
         <f t="array" ref="P61:R61">+ALU!$B$7:$D$7</f>
         <v>1</v>
       </c>
-      <c r="Q61" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="R61" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="S61" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T61" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U61" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="V61" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="W61" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="X61" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y61" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Z61" s="20"/>
-      <c r="AA61" s="23"/>
-      <c r="AB61" s="24"/>
-      <c r="AC61" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q61" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="R61" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S61" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T61" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U61" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="V61" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="W61" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="X61" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y61" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Z61" s="21"/>
+      <c r="AB61" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC61" s="25"/>
       <c r="AD61" s="3"/>
     </row>
     <row r="62">
       <c r="A62" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A62:A63" si="8">CONCATENATE(C62," ",D62,", ",E62)</f>
         <v>NOT B, A</v>
       </c>
       <c r="B62" s="2" t="str">
@@ -14757,185 +14947,182 @@
       <c r="Y62" s="2">
         <v>0.0</v>
       </c>
-      <c r="AA62" s="3"/>
-      <c r="AC62" s="3"/>
+      <c r="AB62" s="3"/>
       <c r="AD62" s="3"/>
     </row>
     <row r="63">
-      <c r="A63" s="20" t="str">
+      <c r="A63" s="21" t="str">
         <f t="shared" si="8"/>
         <v>NOT (Dir), A</v>
       </c>
-      <c r="B63" s="20" t="str">
+      <c r="B63" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00011000001011000001</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E63" s="21" t="s">
+      <c r="E63" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F63" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G63" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H63" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I63" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="J63" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="K63" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L63" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M63" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N63" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O63" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P63" s="20">
+      <c r="F63" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G63" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H63" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I63" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="J63" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="K63" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L63" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M63" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N63" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O63" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P63" s="21">
         <f t="array" ref="P63:R63">+ALU!$B$7:$D$7</f>
         <v>1</v>
       </c>
-      <c r="Q63" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="R63" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="S63" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T63" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U63" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="V63" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="W63" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="X63" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y63" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="Z63" s="20"/>
-      <c r="AA63" s="20"/>
-      <c r="AB63" s="24"/>
-      <c r="AC63" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q63" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="R63" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S63" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T63" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U63" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="V63" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="W63" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="X63" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y63" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="Z63" s="21"/>
+      <c r="AB63" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC63" s="25"/>
       <c r="AD63" s="3"/>
     </row>
     <row r="64">
-      <c r="A64" s="20" t="str">
-        <f t="shared" si="8"/>
-        <v>SHL A, </v>
-      </c>
-      <c r="B64" s="20" t="str">
+      <c r="A64" s="21" t="str">
+        <f>CONCATENATE(C64," ",D64)</f>
+        <v>SHL A</v>
+      </c>
+      <c r="B64" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00000000001101000100</v>
       </c>
-      <c r="C64" s="20" t="s">
+      <c r="C64" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E64" s="21"/>
-      <c r="F64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="J64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="K64" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L64" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M64" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N64" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P64" s="20">
+      <c r="E64" s="22"/>
+      <c r="F64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="J64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="K64" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L64" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M64" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N64" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P64" s="21">
         <f t="array" ref="P64:R64">+ALU!$B$8:$D$8</f>
         <v>1</v>
       </c>
-      <c r="Q64" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="R64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="S64" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="V64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="W64" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="X64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y64" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Z64" s="20"/>
-      <c r="AA64" s="23"/>
-      <c r="AB64" s="24"/>
-      <c r="AC64" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q64" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="R64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="S64" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="V64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="W64" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="X64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y64" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Z64" s="21"/>
+      <c r="AB64" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC64" s="25"/>
       <c r="AD64" s="3"/>
     </row>
     <row r="65">
       <c r="A65" s="2" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="A65:A66" si="9">CONCATENATE(C65," ",D65,", ",E65)</f>
         <v>SHL B, A</v>
       </c>
       <c r="B65" s="2" t="str">
@@ -15012,356 +15199,351 @@
       <c r="Y65" s="2">
         <v>0.0</v>
       </c>
-      <c r="AA65" s="3"/>
-      <c r="AC65" s="3"/>
+      <c r="AB65" s="3"/>
       <c r="AD65" s="3"/>
     </row>
     <row r="66">
-      <c r="A66" s="20" t="str">
-        <f t="shared" si="8"/>
+      <c r="A66" s="21" t="str">
+        <f t="shared" si="9"/>
         <v>SHL (Dir), A</v>
       </c>
-      <c r="B66" s="20" t="str">
+      <c r="B66" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00011000001101000001</v>
       </c>
-      <c r="C66" s="20" t="s">
+      <c r="C66" s="21" t="s">
         <v>43</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E66" s="21" t="s">
+      <c r="E66" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F66" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G66" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H66" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I66" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="J66" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="K66" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L66" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M66" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N66" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O66" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P66" s="20">
+      <c r="F66" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G66" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H66" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I66" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="J66" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="K66" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L66" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M66" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N66" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O66" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P66" s="21">
         <f t="array" ref="P66:R66">+ALU!$B$8:$D$8</f>
         <v>1</v>
       </c>
-      <c r="Q66" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="R66" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="S66" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T66" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U66" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="V66" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="W66" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="X66" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y66" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="Z66" s="20"/>
-      <c r="AA66" s="20"/>
-      <c r="AB66" s="24"/>
-      <c r="AC66" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q66" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="R66" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="S66" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T66" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U66" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="V66" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="W66" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="X66" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y66" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="Z66" s="21"/>
+      <c r="AB66" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC66" s="25"/>
       <c r="AD66" s="3"/>
     </row>
     <row r="67">
-      <c r="A67" s="20" t="str">
-        <f t="shared" si="8"/>
-        <v>SHR A, </v>
-      </c>
-      <c r="B67" s="20" t="str">
+      <c r="A67" s="21" t="str">
+        <f>CONCATENATE(C67," ",D67)</f>
+        <v>SHR A</v>
+      </c>
+      <c r="B67" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00000000001111000100</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D67" s="20" t="s">
+      <c r="D67" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="E67" s="21"/>
-      <c r="F67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="J67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="K67" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L67" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M67" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N67" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P67" s="20">
+      <c r="E67" s="22"/>
+      <c r="F67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="J67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="K67" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L67" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M67" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N67" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P67" s="21">
         <f t="array" ref="P67:R67">+ALU!$B$9:$D$9</f>
         <v>1</v>
       </c>
-      <c r="Q67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="R67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="S67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="V67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="W67" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="X67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y67" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Z67" s="20"/>
-      <c r="AA67" s="23"/>
-      <c r="AB67" s="24"/>
-      <c r="AC67" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q67" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="R67" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S67" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="V67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="W67" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="X67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y67" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Z67" s="21"/>
+      <c r="AB67" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC67" s="25"/>
       <c r="AD67" s="3"/>
     </row>
     <row r="68">
-      <c r="A68" s="20" t="str">
-        <f t="shared" si="8"/>
+      <c r="A68" s="21" t="str">
+        <f t="shared" ref="A68:A69" si="10">CONCATENATE(C68," ",D68,", ",E68)</f>
         <v>SHR B, A</v>
       </c>
-      <c r="B68" s="20" t="str">
+      <c r="B68" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00000000001111000010</v>
       </c>
-      <c r="C68" s="20" t="s">
+      <c r="C68" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D68" s="20" t="s">
+      <c r="D68" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="E68" s="20" t="s">
+      <c r="E68" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="J68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="K68" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L68" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M68" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N68" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O68" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P68" s="20">
+      <c r="F68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="J68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="K68" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L68" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M68" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N68" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O68" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P68" s="21">
         <f t="array" ref="P68:R68">+ALU!$B$9:$D$9</f>
         <v>1</v>
       </c>
-      <c r="Q68" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="R68" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="S68" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T68" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U68" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="V68" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="W68" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="X68" s="21">
-        <v>1.0</v>
-      </c>
-      <c r="Y68" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Z68" s="20"/>
-      <c r="AA68" s="23"/>
-      <c r="AC68" s="3"/>
+      <c r="Q68" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="R68" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S68" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T68" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U68" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="V68" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="W68" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="X68" s="22">
+        <v>1.0</v>
+      </c>
+      <c r="Y68" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Z68" s="21"/>
+      <c r="AB68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
     <row r="69">
-      <c r="A69" s="20" t="str">
-        <f t="shared" si="8"/>
+      <c r="A69" s="21" t="str">
+        <f t="shared" si="10"/>
         <v>SHR (Dir), A</v>
       </c>
-      <c r="B69" s="20" t="str">
+      <c r="B69" s="21" t="str">
         <f t="shared" si="1"/>
         <v>00011000001111000001</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="E69" s="21" t="s">
+      <c r="E69" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="F69" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="G69" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="H69" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="I69" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="J69" s="22">
-        <v>1.0</v>
-      </c>
-      <c r="K69" s="22">
-        <v>0.0</v>
-      </c>
-      <c r="L69" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="M69" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="N69" s="23">
-        <v>0.0</v>
-      </c>
-      <c r="O69" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="P69" s="20">
+      <c r="F69" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="G69" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="H69" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="I69" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="J69" s="23">
+        <v>1.0</v>
+      </c>
+      <c r="K69" s="23">
+        <v>0.0</v>
+      </c>
+      <c r="L69" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="M69" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="N69" s="24">
+        <v>0.0</v>
+      </c>
+      <c r="O69" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="P69" s="21">
         <f t="array" ref="P69:R69">+ALU!$B$9:$D$9</f>
         <v>1</v>
       </c>
-      <c r="Q69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="R69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="S69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="T69" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="U69" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="V69" s="21">
-        <v>0.0</v>
-      </c>
-      <c r="W69" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="X69" s="20">
-        <v>0.0</v>
-      </c>
-      <c r="Y69" s="20">
-        <v>1.0</v>
-      </c>
-      <c r="Z69" s="20"/>
-      <c r="AA69" s="20"/>
-      <c r="AB69" s="24"/>
-      <c r="AC69" s="9" t="s">
-        <v>77</v>
-      </c>
+      <c r="Q69" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="R69" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="S69" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="T69" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="U69" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="V69" s="22">
+        <v>0.0</v>
+      </c>
+      <c r="W69" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="X69" s="21">
+        <v>0.0</v>
+      </c>
+      <c r="Y69" s="21">
+        <v>1.0</v>
+      </c>
+      <c r="Z69" s="21"/>
+      <c r="AB69" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC69" s="25"/>
       <c r="AD69" s="3"/>
     </row>
     <row r="70">
       <c r="A70" s="15" t="str">
-        <f>CONCATENATE(C70," ",D70)</f>
+        <f t="shared" ref="A70:A74" si="11">CONCATENATE(C70," ",D70)</f>
         <v>INC A</v>
       </c>
       <c r="B70" s="15" t="str">
@@ -15420,8 +15602,8 @@
       <c r="T70" s="16">
         <v>0.0</v>
       </c>
-      <c r="U70" s="25"/>
-      <c r="V70" s="25"/>
+      <c r="U70" s="26"/>
+      <c r="V70" s="26"/>
       <c r="W70" s="15">
         <v>1.0</v>
       </c>
@@ -15431,20 +15613,18 @@
       <c r="Y70" s="15">
         <v>0.0</v>
       </c>
-      <c r="Z70" s="26" t="s">
-        <v>78</v>
-      </c>
-      <c r="AA70" s="15"/>
-      <c r="AB70" s="11" t="s">
+      <c r="AB70" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="AC70" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
     </row>
     <row r="71">
       <c r="A71" s="2" t="str">
-        <f t="shared" ref="A71:A73" si="9">CONCATENATE(C71," ",D71,", ",E71)</f>
-        <v>INC B, </v>
+        <f t="shared" si="11"/>
+        <v>INC B</v>
       </c>
       <c r="B71" s="2" t="str">
         <f t="shared" si="1"/>
@@ -15498,7 +15678,7 @@
       <c r="S71" s="27">
         <v>1.0</v>
       </c>
-      <c r="T71" s="24">
+      <c r="T71" s="25">
         <v>1.0</v>
       </c>
       <c r="U71" s="2">
@@ -15516,16 +15696,15 @@
       <c r="Y71" s="2">
         <v>0.0</v>
       </c>
-      <c r="Z71" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AC71" s="3"/>
+      <c r="AB71" s="1" t="s">
+        <v>83</v>
+      </c>
       <c r="AD71" s="3"/>
     </row>
     <row r="72">
       <c r="A72" s="12" t="str">
-        <f t="shared" si="9"/>
-        <v>INC (Dir), </v>
+        <f t="shared" si="11"/>
+        <v>INC (Dir)</v>
       </c>
       <c r="B72" s="12" t="str">
         <f t="shared" si="1"/>
@@ -15577,16 +15756,16 @@
       <c r="R72" s="12">
         <v>0.0</v>
       </c>
-      <c r="S72" s="24">
-        <v>0.0</v>
-      </c>
-      <c r="T72" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="U72" s="24">
-        <v>1.0</v>
-      </c>
-      <c r="V72" s="24">
+      <c r="S72" s="25">
+        <v>0.0</v>
+      </c>
+      <c r="T72" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="U72" s="25">
+        <v>1.0</v>
+      </c>
+      <c r="V72" s="25">
         <v>1.0</v>
       </c>
       <c r="W72" s="12">
@@ -15598,20 +15777,18 @@
       <c r="Y72" s="12">
         <v>1.0</v>
       </c>
-      <c r="Z72" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AA72" s="12"/>
       <c r="AB72" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AC72" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
     </row>
     <row r="73">
       <c r="A73" s="12" t="str">
-        <f t="shared" si="9"/>
-        <v>INC (B), </v>
+        <f t="shared" si="11"/>
+        <v>INC (B)</v>
       </c>
       <c r="B73" s="12" t="str">
         <f t="shared" si="1"/>
@@ -15621,7 +15798,7 @@
         <v>45</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="E73" s="12"/>
       <c r="F73" s="13">
@@ -15670,21 +15847,19 @@
       <c r="W73" s="12"/>
       <c r="X73" s="12"/>
       <c r="Y73" s="12"/>
-      <c r="Z73" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AA73" s="12"/>
       <c r="AB73" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AC73" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC73" s="28"/>
       <c r="AD73" s="28"/>
       <c r="AE73" s="29"/>
       <c r="AF73" s="29"/>
     </row>
     <row r="74">
       <c r="A74" s="12" t="str">
-        <f>CONCATENATE(C74," ",D74)</f>
+        <f t="shared" si="11"/>
         <v>DEC A</v>
       </c>
       <c r="B74" s="12" t="str">
@@ -15743,10 +15918,10 @@
       <c r="T74" s="8">
         <v>0.0</v>
       </c>
-      <c r="U74" s="25">
-        <v>1.0</v>
-      </c>
-      <c r="V74" s="25">
+      <c r="U74" s="26">
+        <v>1.0</v>
+      </c>
+      <c r="V74" s="26">
         <v>1.0</v>
       </c>
       <c r="W74" s="12">
@@ -15758,19 +15933,17 @@
       <c r="Y74" s="12">
         <v>0.0</v>
       </c>
-      <c r="Z74" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA74" s="12"/>
       <c r="AB74" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AC74" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
     </row>
     <row r="75">
       <c r="A75" s="2" t="str">
-        <f t="shared" ref="A75:A78" si="10">CONCATENATE(C75," ",D75,", ",E75)</f>
+        <f t="shared" ref="A75:A78" si="12">CONCATENATE(C75," ",D75,", ",E75)</f>
         <v>CMP A, B</v>
       </c>
       <c r="B75" s="2" t="str">
@@ -15846,12 +16019,12 @@
       <c r="Y75" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC75" s="3"/>
+      <c r="AA75" s="3"/>
       <c r="AD75" s="3"/>
     </row>
     <row r="76">
       <c r="A76" s="2" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>CMP A, Lit</v>
       </c>
       <c r="B76" s="2" t="str">
@@ -15927,12 +16100,12 @@
       <c r="Y76" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC76" s="3"/>
+      <c r="AA76" s="3"/>
       <c r="AD76" s="3"/>
     </row>
     <row r="77">
       <c r="A77" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>CMP A, (Dir)</v>
       </c>
       <c r="B77" s="12" t="str">
@@ -16009,16 +16182,16 @@
         <v>0.0</v>
       </c>
       <c r="Z77" s="12"/>
-      <c r="AA77" s="12"/>
-      <c r="AB77" s="11" t="s">
+      <c r="AA77" s="3"/>
+      <c r="AB77" s="12"/>
+      <c r="AC77" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AC77" s="3"/>
       <c r="AD77" s="3"/>
     </row>
     <row r="78">
       <c r="A78" s="12" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>CMP A, (B)</v>
       </c>
       <c r="B78" s="12" t="str">
@@ -16032,7 +16205,7 @@
         <v>28</v>
       </c>
       <c r="E78" s="11" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F78" s="13">
         <v>0.0</v>
@@ -16081,14 +16254,14 @@
       <c r="X78" s="12"/>
       <c r="Y78" s="12"/>
       <c r="Z78" s="12"/>
-      <c r="AA78" s="12"/>
-      <c r="AB78" s="11"/>
-      <c r="AC78" s="3"/>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="12"/>
+      <c r="AC78" s="11"/>
       <c r="AD78" s="3"/>
     </row>
     <row r="79">
       <c r="A79" s="2" t="str">
-        <f t="shared" ref="A79:A86" si="11">CONCATENATE(C79," ",D79)</f>
+        <f t="shared" ref="A79:A86" si="13">CONCATENATE(C79," ",D79)</f>
         <v>JMP Ins</v>
       </c>
       <c r="B79" s="2" t="str">
@@ -16161,12 +16334,15 @@
       <c r="Y79" s="2">
         <v>0.0</v>
       </c>
-      <c r="AC79" s="3"/>
+      <c r="Z79" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AA79" s="3"/>
       <c r="AD79" s="3"/>
     </row>
     <row r="80">
       <c r="A80" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JEQ Ins</v>
       </c>
       <c r="B80" s="2" t="str">
@@ -16239,13 +16415,13 @@
       <c r="Y80" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB80" s="3"/>
+      <c r="AA80" s="3"/>
       <c r="AC80" s="3"/>
       <c r="AD80" s="3"/>
     </row>
     <row r="81">
       <c r="A81" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JNE Ins</v>
       </c>
       <c r="B81" s="2" t="str">
@@ -16318,13 +16494,13 @@
       <c r="Y81" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB81" s="3"/>
+      <c r="AA81" s="3"/>
       <c r="AC81" s="3"/>
       <c r="AD81" s="3"/>
     </row>
     <row r="82">
       <c r="A82" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JGT Ins</v>
       </c>
       <c r="B82" s="2" t="str">
@@ -16397,13 +16573,13 @@
       <c r="Y82" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB82" s="3"/>
+      <c r="AA82" s="3"/>
       <c r="AC82" s="3"/>
       <c r="AD82" s="3"/>
     </row>
     <row r="83">
       <c r="A83" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JLT Ins</v>
       </c>
       <c r="B83" s="2" t="str">
@@ -16476,13 +16652,13 @@
       <c r="Y83" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB83" s="3"/>
+      <c r="AA83" s="3"/>
       <c r="AC83" s="3"/>
       <c r="AD83" s="3"/>
     </row>
     <row r="84">
       <c r="A84" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JGE Ins</v>
       </c>
       <c r="B84" s="2" t="str">
@@ -16555,13 +16731,13 @@
       <c r="Y84" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB84" s="3"/>
+      <c r="AA84" s="3"/>
       <c r="AC84" s="3"/>
       <c r="AD84" s="3"/>
     </row>
     <row r="85">
       <c r="A85" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JLE Ins</v>
       </c>
       <c r="B85" s="2" t="str">
@@ -16634,13 +16810,13 @@
       <c r="Y85" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB85" s="3"/>
+      <c r="AA85" s="3"/>
       <c r="AC85" s="3"/>
       <c r="AD85" s="3"/>
     </row>
     <row r="86">
       <c r="A86" s="2" t="str">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>JCR Ins</v>
       </c>
       <c r="B86" s="2" t="str">
@@ -16713,23 +16889,23 @@
       <c r="Y86" s="2">
         <v>0.0</v>
       </c>
-      <c r="AB86" s="3"/>
+      <c r="AA86" s="3"/>
       <c r="AC86" s="3"/>
       <c r="AD86" s="3"/>
     </row>
     <row r="87">
       <c r="A87" s="1" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="B87" s="2" t="str">
         <f t="shared" si="1"/>
         <v>10100100000000000001</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>84</v>
+        <v>89</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F87" s="1">
         <v>1.0</v>
@@ -16794,14 +16970,14 @@
     </row>
     <row r="88">
       <c r="A88" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="B88" s="2" t="str">
         <f t="shared" si="1"/>
         <v>01000000000000000000</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="F88" s="1">
         <v>0.0</v>
@@ -16863,8 +17039,8 @@
       <c r="Y88" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z88" s="1" t="s">
-        <v>87</v>
+      <c r="AB88" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="89">
@@ -16932,20 +17108,20 @@
       <c r="Y89" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z89" s="1" t="s">
-        <v>88</v>
+      <c r="AB89" s="1" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="1" t="s">
-        <v>89</v>
+        <v>94</v>
       </c>
       <c r="B90" s="2" t="str">
         <f t="shared" si="1"/>
         <v>10010100000000000001</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>28</v>
@@ -17013,14 +17189,14 @@
     </row>
     <row r="91">
       <c r="A91" s="1" t="s">
-        <v>91</v>
+        <v>96</v>
       </c>
       <c r="B91" s="2" t="str">
         <f t="shared" si="1"/>
         <v>10010100000000010001</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>90</v>
+        <v>95</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>29</v>
@@ -17088,14 +17264,14 @@
     </row>
     <row r="92">
       <c r="A92" s="1" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="B92" s="2" t="str">
         <f t="shared" si="1"/>
         <v>01000000000000000000</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>28</v>
@@ -17160,8 +17336,8 @@
       <c r="Y92" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z92" s="1" t="s">
-        <v>87</v>
+      <c r="AB92" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="93">
@@ -17229,20 +17405,20 @@
       <c r="Y93" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z93" s="1" t="s">
-        <v>94</v>
+      <c r="AB93" s="1" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="1" t="s">
-        <v>95</v>
+        <v>100</v>
       </c>
       <c r="B94" s="2" t="str">
         <f t="shared" si="1"/>
         <v>01000000000000000000</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>93</v>
+        <v>98</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>29</v>
@@ -17307,8 +17483,8 @@
       <c r="Y94" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z94" s="1" t="s">
-        <v>87</v>
+      <c r="AB94" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="95">
@@ -17376,8 +17552,8 @@
       <c r="Y95" s="1">
         <v>0.0</v>
       </c>
-      <c r="Z95" s="1" t="s">
-        <v>96</v>
+      <c r="AB95" s="1" t="s">
+        <v>101</v>
       </c>
     </row>
     <row r="97">
@@ -17385,7 +17561,7 @@
         <v>1.0</v>
       </c>
       <c r="I97" s="1" t="s">
-        <v>97</v>
+        <v>102</v>
       </c>
       <c r="J97" s="32">
         <v>0.0</v>
@@ -17394,7 +17570,7 @@
         <v>0.0</v>
       </c>
       <c r="L97" s="32" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98">
@@ -17402,7 +17578,7 @@
         <v>0.0</v>
       </c>
       <c r="I98" s="1" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="J98" s="32">
         <v>1.0</v>
@@ -17437,6 +17613,11 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="Z12:AA15">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>SI</formula>
+    </cfRule>
+  </conditionalFormatting>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
@@ -17460,7 +17641,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>18</v>
@@ -17469,15 +17650,15 @@
         <v>19</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B2" s="2">
         <v>0.0</v>
@@ -17486,7 +17667,7 @@
         <v>0.0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F2" s="1">
         <v>1.0</v>
@@ -17494,7 +17675,7 @@
     </row>
     <row r="3">
       <c r="A3" s="2" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B3" s="2">
         <v>0.0</v>
@@ -17503,7 +17684,7 @@
         <v>1.0</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>106</v>
+        <v>111</v>
       </c>
       <c r="F3" s="1">
         <v>0.0</v>
@@ -17511,7 +17692,7 @@
     </row>
     <row r="4">
       <c r="A4" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B4" s="2">
         <v>1.0</v>
@@ -17522,7 +17703,7 @@
     </row>
     <row r="5">
       <c r="A5" s="8" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B5" s="8">
         <v>1.0</v>
@@ -17531,18 +17712,18 @@
         <v>1.0</v>
       </c>
       <c r="E5" s="32" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="F5" s="32" t="s">
-        <v>110</v>
+        <v>115</v>
       </c>
       <c r="G5" s="32" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6">
       <c r="E6" s="32" t="s">
-        <v>104</v>
+        <v>109</v>
       </c>
       <c r="F6" s="32">
         <v>1.0</v>
@@ -17553,7 +17734,7 @@
     </row>
     <row r="7">
       <c r="E7" s="32" t="s">
-        <v>112</v>
+        <v>117</v>
       </c>
       <c r="F7" s="32">
         <v>1.0</v>
@@ -17564,7 +17745,7 @@
     </row>
     <row r="8">
       <c r="A8" s="2" t="s">
-        <v>113</v>
+        <v>118</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>20</v>
@@ -17584,7 +17765,7 @@
     </row>
     <row r="9">
       <c r="A9" s="2" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
       <c r="B9" s="2">
         <v>0.0</v>
@@ -17593,7 +17774,7 @@
         <v>0.0</v>
       </c>
       <c r="E9" s="32" t="s">
-        <v>114</v>
+        <v>119</v>
       </c>
       <c r="F9" s="32">
         <v>0.0</v>
@@ -17604,7 +17785,7 @@
     </row>
     <row r="10">
       <c r="A10" s="2" t="s">
-        <v>108</v>
+        <v>113</v>
       </c>
       <c r="B10" s="2">
         <v>0.0</v>
@@ -17615,7 +17796,7 @@
     </row>
     <row r="11">
       <c r="A11" s="2" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B11" s="2">
         <v>1.0</v>
@@ -17624,15 +17805,15 @@
         <v>0.0</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="s">
-        <v>118</v>
+        <v>123</v>
       </c>
       <c r="B12" s="2">
         <v>1.0</v>
@@ -17641,7 +17822,7 @@
         <v>1.0</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>119</v>
+        <v>124</v>
       </c>
       <c r="F12" s="1">
         <v>1.0</v>
@@ -17649,7 +17830,7 @@
     </row>
     <row r="13">
       <c r="E13" s="1" t="s">
-        <v>120</v>
+        <v>125</v>
       </c>
       <c r="F13" s="1">
         <v>0.0</v>
@@ -17657,7 +17838,7 @@
     </row>
     <row r="14">
       <c r="A14" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>22</v>
@@ -17665,7 +17846,7 @@
     </row>
     <row r="15">
       <c r="A15" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B15" s="2">
         <v>0.0</v>
@@ -17673,7 +17854,7 @@
     </row>
     <row r="16">
       <c r="A16" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B16" s="2">
         <v>1.0</v>
@@ -17681,7 +17862,7 @@
     </row>
     <row r="18">
       <c r="A18" s="2" t="s">
-        <v>107</v>
+        <v>112</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>23</v>
@@ -17689,7 +17870,7 @@
     </row>
     <row r="19">
       <c r="A19" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B19" s="2">
         <v>0.0</v>
@@ -17697,7 +17878,7 @@
     </row>
     <row r="20">
       <c r="A20" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B20" s="2">
         <v>1.0</v>
@@ -17706,15 +17887,15 @@
     <row r="21" ht="15.75" customHeight="1"/>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="1" t="s">
-        <v>123</v>
+        <v>128</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>124</v>
+        <v>129</v>
       </c>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="2" t="s">
-        <v>121</v>
+        <v>126</v>
       </c>
       <c r="B23" s="2">
         <v>0.0</v>
@@ -17722,7 +17903,7 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="2" t="s">
-        <v>122</v>
+        <v>127</v>
       </c>
       <c r="B24" s="2">
         <v>1.0</v>
@@ -18727,7 +18908,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="2" t="s">
-        <v>125</v>
+        <v>130</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>15</v>

</xml_diff>